<commit_message>
Update files to EN Console
</commit_message>
<xml_diff>
--- a/console/Hyper-Converged-IDC/HyperConvergedIDC-CPS-控制台翻译内容-1116补充.xlsx
+++ b/console/Hyper-Converged-IDC/HyperConvergedIDC-CPS-控制台翻译内容-1116补充.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -40,10 +40,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Exceed accumulative purchase quantity of the user. Please adjust the purchase quantity.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -56,181 +52,185 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>目前暂不对个人认证用户开放低价折扣优惠活动，请静待后续活动，或在用户管理页面升级为企业用户。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>购买数量超限</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>活动期间仅限购买</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>台云物理服务器</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only 1 Cloud Physical Server can be purchased during the promotion.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>存在未支付订单</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orders Unpaid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>您有未支付订单，请在订单管理页面支付未支付订单</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>开机成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>关机成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shutdown Succeeded</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>重启成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reboot Succeeded</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>已取消</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Canceled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exceed purchase quantity limit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exceed user's accumulative purchase quantity, please adjust.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>At present, high discount promotion is not opened to certified individual users. Please wait for later promotions or upgrade to be an enterprise user on the User Management Page.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You have order(s) unpaid. Please pay on the Order Management Page.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Exceed user's accumulative purchase quantity </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Individual User Not Supported</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>目前暂不对个人认证用户开放低价折扣优惠活动，请静待后续活动，或在用户管理页面升级为企业用户。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>购买数量超限</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>活动期间仅限购买</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>台云物理服务器</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Only 1 Cloud Physical Server can be purchased during the promotion.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>存在未支付订单</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Orders Unpaid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>您有未支付订单，请在订单管理页面支付未支付订单</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>You have the order(s) unpaid. Please pay the orders in the order management page.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>开机成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Startup Succeeded</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>关机成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shutdown Succeeded</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>重启成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reboot Succeeded</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-      </rPr>
-      <t>已取消</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Canceled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exceed accumulative purchase quantity of the user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>At present, the high discount promotion has not been opened to the certified individual user. Please wait for other promotions or upgrade to be the enterprise user in the user management page.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exceed purchase quantity limit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,20 +564,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="65.25" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -585,93 +585,96 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="42.75">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="28.5">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>